<commit_message>
Final Changes Si Teng
</commit_message>
<xml_diff>
--- a/Main/triTest.xlsx
+++ b/Main/triTest.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,6 +446,11 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Percentage Error</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Pass/Fail</t>
         </is>
       </c>
@@ -461,12 +466,15 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.5000000000000299,0.5000000000001981</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Fail</t>
+          <t>0.5000000000057143,0.19999999999224918</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>1.02073315838368e-09</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Pass</t>
         </is>
       </c>
     </row>

</xml_diff>